<commit_message>
YTI-696: Correcting integration test data and adding support for new error message along with an implementation bugfix to resolving relations.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_exttest_codescheme.xlsx
+++ b/src/test/resources/codeschemes/v1_exttest_codescheme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4019C5A7-5967-DB40-9826-34EF48D1CCF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79B8982-766B-204D-BBA3-A46B092E1630}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="Members_exttest_test-1" sheetId="5" r:id="rId5"/>
     <sheet name="Members_exttest_test-2" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="314">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -955,13 +955,25 @@
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/testregistry1/exttest/code/testcode10</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/testregistry1/exttest/extension/test-1/member/7</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/testregistry1/exttest/extension/test-1/member/8</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/testregistry1/exttest/extension/test-1/member/1</t>
+  </si>
+  <si>
+    <t>http://uri.suomi.fi/codelist/testregistry1/exttest/extension/test-1/member/5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -973,6 +985,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1319,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3126,15 +3144,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -3182,9 +3200,6 @@
       <c r="D2" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
@@ -3215,7 +3230,7 @@
         <v>281</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="F3" t="s">
         <v>45</v>
@@ -3246,8 +3261,8 @@
       <c r="D4" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E4">
-        <v>4</v>
+      <c r="E4" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="F4" t="s">
         <v>45</v>
@@ -3278,8 +3293,8 @@
       <c r="D5" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E5" t="s">
-        <v>123</v>
+      <c r="E5" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="F5" t="s">
         <v>45</v>
@@ -3310,8 +3325,8 @@
       <c r="D6" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E6">
-        <v>6</v>
+      <c r="E6" t="s">
+        <v>99</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -3342,8 +3357,8 @@
       <c r="D7" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E7">
-        <v>7</v>
+      <c r="E7" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="F7" t="s">
         <v>45</v>
@@ -3374,8 +3389,8 @@
       <c r="D8" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E8">
-        <v>8</v>
+      <c r="E8" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
@@ -3406,8 +3421,8 @@
       <c r="D9" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E9">
-        <v>9</v>
+      <c r="E9" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="F9" t="s">
         <v>45</v>
@@ -3438,8 +3453,8 @@
       <c r="D10" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E10">
-        <v>10</v>
+      <c r="E10" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="F10" t="s">
         <v>45</v>
@@ -3471,7 +3486,7 @@
         <v>289</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="F11" t="s">
         <v>45</v>
@@ -3503,7 +3518,7 @@
         <v>290</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F12" t="s">
         <v>45</v>
@@ -3534,6 +3549,9 @@
       <c r="D13" s="1" t="s">
         <v>291</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>280</v>
+      </c>
       <c r="F13" t="s">
         <v>45</v>
       </c>
@@ -3563,8 +3581,8 @@
       <c r="D14" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E14" t="s">
-        <v>45</v>
+      <c r="E14" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="F14" t="s">
         <v>45</v>
@@ -3597,10 +3615,17 @@
     <hyperlink ref="D12" r:id="rId11" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode21" xr:uid="{28499826-0108-1E48-8CE4-7B6BBDC671DA}"/>
     <hyperlink ref="D13" r:id="rId12" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode23" xr:uid="{E014DFCC-89F1-BC4E-BDDD-E6CEDD2C490C}"/>
     <hyperlink ref="D14" r:id="rId13" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode25" xr:uid="{504729AD-6C44-8E43-87AC-5702E8C10C87}"/>
-    <hyperlink ref="E3" r:id="rId14" display="http://uri.suomi.fi/codelist/test/exttest/extension/test-1/member/3" xr:uid="{2F98DB0B-B700-8042-8834-5815E634B25B}"/>
-    <hyperlink ref="E12" r:id="rId15" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode23" xr:uid="{6393BAA2-B138-7B46-8133-24B013B8DC02}"/>
-    <hyperlink ref="E11" r:id="rId16" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode21" xr:uid="{B33501CF-5F82-5F43-8BDB-55B2798EE36B}"/>
-    <hyperlink ref="E2" r:id="rId17" display="http://uri.suomi.fi/codelist/test/exttest/extension/test-1/member/2" xr:uid="{75ACF0A2-429E-8F44-9A1A-58C8F440F2DC}"/>
+    <hyperlink ref="E4" r:id="rId14" xr:uid="{2F98DB0B-B700-8042-8834-5815E634B25B}"/>
+    <hyperlink ref="E13" r:id="rId15" xr:uid="{6393BAA2-B138-7B46-8133-24B013B8DC02}"/>
+    <hyperlink ref="E12" r:id="rId16" xr:uid="{B33501CF-5F82-5F43-8BDB-55B2798EE36B}"/>
+    <hyperlink ref="E3" r:id="rId17" xr:uid="{75ACF0A2-429E-8F44-9A1A-58C8F440F2DC}"/>
+    <hyperlink ref="E5" r:id="rId18" xr:uid="{5BF235B2-1212-1F44-95D3-A4A36274C9A5}"/>
+    <hyperlink ref="E7" r:id="rId19" xr:uid="{F57F06A8-7663-704A-93C7-E85D624E57B3}"/>
+    <hyperlink ref="E8" r:id="rId20" xr:uid="{6F6ADED1-832B-B947-B70B-4B4463A2DEBC}"/>
+    <hyperlink ref="E9" r:id="rId21" xr:uid="{1CD60424-C869-0346-93E7-87DFE5436EBF}"/>
+    <hyperlink ref="E10" r:id="rId22" xr:uid="{B3D15CCB-71F2-E847-9E32-BE9FBEF2B0C1}"/>
+    <hyperlink ref="E11" r:id="rId23" xr:uid="{7911ECD0-047A-C242-A1DB-7BB53C6D844D}"/>
+    <hyperlink ref="E14" r:id="rId24" xr:uid="{7744A89E-F567-064C-B59B-D30E6C221E1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3611,13 +3636,14 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="58.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -3724,8 +3750,8 @@
       <c r="G3" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="H3" t="s">
-        <v>79</v>
+      <c r="H3" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="I3" t="s">
         <v>45</v>
@@ -3765,8 +3791,8 @@
       <c r="G4" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="H4" t="s">
-        <v>85</v>
+      <c r="H4" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="I4" t="s">
         <v>45</v>
@@ -3806,8 +3832,8 @@
       <c r="G5" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="H5" t="s">
-        <v>92</v>
+      <c r="H5" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="I5" t="s">
         <v>45</v>
@@ -3847,8 +3873,8 @@
       <c r="G6" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="H6" t="s">
-        <v>98</v>
+      <c r="H6" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="I6" t="s">
         <v>45</v>
@@ -3888,8 +3914,8 @@
       <c r="G7" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="H7" t="s">
-        <v>104</v>
+      <c r="H7" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="I7" t="s">
         <v>45</v>
@@ -3929,8 +3955,8 @@
       <c r="G8" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="H8" t="s">
-        <v>110</v>
+      <c r="H8" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="I8" t="s">
         <v>45</v>
@@ -3970,8 +3996,8 @@
       <c r="G9" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H9" t="s">
-        <v>116</v>
+      <c r="H9" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="I9" t="s">
         <v>45</v>
@@ -4011,8 +4037,8 @@
       <c r="G10" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="H10" t="s">
-        <v>122</v>
+      <c r="H10" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="I10" t="s">
         <v>45</v>
@@ -4052,8 +4078,8 @@
       <c r="G11" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="H11" t="s">
-        <v>128</v>
+      <c r="H11" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="I11" t="s">
         <v>45</v>
@@ -4072,6 +4098,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode01" xr:uid="{D8AA95B2-E723-A249-900E-6D3B5EF07CE5}"/>
     <hyperlink ref="G3" r:id="rId2" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode02" xr:uid="{72020926-C7A2-6148-B6A7-17AB2E00D76A}"/>
@@ -4093,6 +4120,8 @@
     <hyperlink ref="B9" r:id="rId18" display="http://uri.suomi.fi/codelist/test/exttest/extension/test-2/member/8" xr:uid="{32B2FD3A-881D-B94A-8422-FEEDB65E2B03}"/>
     <hyperlink ref="B10" r:id="rId19" display="http://uri.suomi.fi/codelist/test/exttest/extension/test-2/member/9" xr:uid="{8F16FE5E-608A-D846-BD77-D627C28EAA81}"/>
     <hyperlink ref="B11" r:id="rId20" display="http://uri.suomi.fi/codelist/test/exttest/extension/test-2/member/10" xr:uid="{0AA094B8-DA65-734B-BE23-112DD385F03C}"/>
+    <hyperlink ref="H3" r:id="rId21" xr:uid="{03D0D902-9F50-134A-9B0D-D1ED70B6B7F8}"/>
+    <hyperlink ref="H4:H11" r:id="rId22" display="http://uri.suomi.fi/codelist/testregistry1/exttest/extension/test-2/member/1" xr:uid="{8395588E-3D9D-094A-90C1-0347824D8066}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
YTI-696: Member relation importing refactored to support code: and member: prefix. Default non-prefixed value is evaluated as member sequence id.
</commit_message>
<xml_diff>
--- a/src/test/resources/codeschemes/v1_exttest_codescheme.xlsx
+++ b/src/test/resources/codeschemes/v1_exttest_codescheme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antti.tohmo/Projects/yti/yti-codelist-content-intake-service/src/test/resources/codeschemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79B8982-766B-204D-BBA3-A46B092E1630}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B457C53-113D-4E46-8D30-7B0E84F06B52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="315">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -906,9 +906,6 @@
     <t>http://uri.suomi.fi/codelist/testregistry1/exttest/code/testcode25</t>
   </si>
   <si>
-    <t>http://uri.suomi.fi/codelist/testregistry1/exttest/extension/test-1/member/2</t>
-  </si>
-  <si>
     <t>http://uri.suomi.fi/codelist/testregistry1/exttest/extension/test-1/member/3</t>
   </si>
   <si>
@@ -967,13 +964,19 @@
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/testregistry1/exttest/extension/test-1/member/5</t>
+  </si>
+  <si>
+    <t>code:testcode05</t>
+  </si>
+  <si>
+    <t>member:3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -991,6 +994,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1017,9 +1027,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3145,7 +3157,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3197,8 +3209,8 @@
       <c r="C2" t="s">
         <v>239</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>280</v>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
@@ -3226,11 +3238,11 @@
       <c r="C3" t="s">
         <v>242</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>312</v>
+      <c r="D3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="F3" t="s">
         <v>45</v>
@@ -3258,11 +3270,11 @@
       <c r="C4" t="s">
         <v>244</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>293</v>
+      <c r="D4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
       </c>
       <c r="F4" t="s">
         <v>45</v>
@@ -3290,11 +3302,11 @@
       <c r="C5" t="s">
         <v>246</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>294</v>
+      <c r="E5" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="F5" t="s">
         <v>45</v>
@@ -3322,11 +3334,11 @@
       <c r="C6" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>284</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>313</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -3354,11 +3366,11 @@
       <c r="C7" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>313</v>
+      <c r="E7" s="2" t="s">
+        <v>312</v>
       </c>
       <c r="F7" t="s">
         <v>45</v>
@@ -3386,11 +3398,11 @@
       <c r="C8" t="s">
         <v>252</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>313</v>
+      <c r="E8" s="2" t="s">
+        <v>312</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
@@ -3418,11 +3430,11 @@
       <c r="C9" t="s">
         <v>254</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>313</v>
+      <c r="E9" s="2" t="s">
+        <v>312</v>
       </c>
       <c r="F9" t="s">
         <v>45</v>
@@ -3450,11 +3462,11 @@
       <c r="C10" t="s">
         <v>256</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>310</v>
+      <c r="E10" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="F10" t="s">
         <v>45</v>
@@ -3482,11 +3494,11 @@
       <c r="C11" t="s">
         <v>258</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>311</v>
+      <c r="E11" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="F11" t="s">
         <v>45</v>
@@ -3514,10 +3526,10 @@
       <c r="C12" t="s">
         <v>260</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>288</v>
       </c>
       <c r="F12" t="s">
@@ -3546,10 +3558,10 @@
       <c r="C13" t="s">
         <v>262</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>280</v>
       </c>
       <c r="F13" t="s">
@@ -3578,11 +3590,11 @@
       <c r="C14" t="s">
         <v>265</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>294</v>
+      <c r="E14" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="F14" t="s">
         <v>45</v>
@@ -3601,32 +3613,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode01" xr:uid="{850571D3-4D61-A447-936F-27890D275D1B}"/>
-    <hyperlink ref="D3" r:id="rId2" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode03" xr:uid="{F8538B4C-31CC-584A-81EE-27A000B998B4}"/>
-    <hyperlink ref="D4" r:id="rId3" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode05" xr:uid="{79C44080-8701-794C-8AD0-E1FCA2AE876E}"/>
-    <hyperlink ref="D5" r:id="rId4" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode07" xr:uid="{4B176178-8893-2648-B9E0-9BBBB1C3C572}"/>
-    <hyperlink ref="D6" r:id="rId5" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode09" xr:uid="{6FD235A1-3DD5-5B4B-A5BE-2B2669ED4FD9}"/>
-    <hyperlink ref="D7" r:id="rId6" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode11" xr:uid="{7F829F38-E86A-7C4B-8318-83C07DA36AE0}"/>
-    <hyperlink ref="D8" r:id="rId7" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode13" xr:uid="{3EBF1A33-5F89-ED43-BCB8-736C06C838EF}"/>
-    <hyperlink ref="D9" r:id="rId8" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode15" xr:uid="{74CD5366-70D8-AC4D-9A05-2789A4AC956F}"/>
-    <hyperlink ref="D10" r:id="rId9" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode17" xr:uid="{97CEA41F-4573-F846-BF37-330A69DD673A}"/>
-    <hyperlink ref="D11" r:id="rId10" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode19" xr:uid="{D0066006-72B7-BC4F-A78A-28A0345FC485}"/>
-    <hyperlink ref="D12" r:id="rId11" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode21" xr:uid="{28499826-0108-1E48-8CE4-7B6BBDC671DA}"/>
-    <hyperlink ref="D13" r:id="rId12" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode23" xr:uid="{E014DFCC-89F1-BC4E-BDDD-E6CEDD2C490C}"/>
-    <hyperlink ref="D14" r:id="rId13" display="http://uri.suomi.fi/codelist/test/exttest/code/testcode25" xr:uid="{504729AD-6C44-8E43-87AC-5702E8C10C87}"/>
-    <hyperlink ref="E4" r:id="rId14" xr:uid="{2F98DB0B-B700-8042-8834-5815E634B25B}"/>
-    <hyperlink ref="E13" r:id="rId15" xr:uid="{6393BAA2-B138-7B46-8133-24B013B8DC02}"/>
-    <hyperlink ref="E12" r:id="rId16" xr:uid="{B33501CF-5F82-5F43-8BDB-55B2798EE36B}"/>
-    <hyperlink ref="E3" r:id="rId17" xr:uid="{75ACF0A2-429E-8F44-9A1A-58C8F440F2DC}"/>
-    <hyperlink ref="E5" r:id="rId18" xr:uid="{5BF235B2-1212-1F44-95D3-A4A36274C9A5}"/>
-    <hyperlink ref="E7" r:id="rId19" xr:uid="{F57F06A8-7663-704A-93C7-E85D624E57B3}"/>
-    <hyperlink ref="E8" r:id="rId20" xr:uid="{6F6ADED1-832B-B947-B70B-4B4463A2DEBC}"/>
-    <hyperlink ref="E9" r:id="rId21" xr:uid="{1CD60424-C869-0346-93E7-87DFE5436EBF}"/>
-    <hyperlink ref="E10" r:id="rId22" xr:uid="{B3D15CCB-71F2-E847-9E32-BE9FBEF2B0C1}"/>
-    <hyperlink ref="E11" r:id="rId23" xr:uid="{7911ECD0-047A-C242-A1DB-7BB53C6D844D}"/>
-    <hyperlink ref="E14" r:id="rId24" xr:uid="{7744A89E-F567-064C-B59B-D30E6C221E1C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3692,7 +3678,7 @@
         <v>79</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C2" t="s">
         <v>269</v>
@@ -3733,7 +3719,7 @@
         <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
         <v>269</v>
@@ -3748,10 +3734,10 @@
         <v>242</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I3" t="s">
         <v>45</v>
@@ -3774,7 +3760,7 @@
         <v>92</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C4" t="s">
         <v>269</v>
@@ -3792,7 +3778,7 @@
         <v>281</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I4" t="s">
         <v>45</v>
@@ -3815,7 +3801,7 @@
         <v>98</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C5" t="s">
         <v>269</v>
@@ -3830,10 +3816,10 @@
         <v>246</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I5" t="s">
         <v>45</v>
@@ -3856,7 +3842,7 @@
         <v>104</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C6" t="s">
         <v>269</v>
@@ -3874,7 +3860,7 @@
         <v>282</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I6" t="s">
         <v>45</v>
@@ -3897,7 +3883,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C7" t="s">
         <v>269</v>
@@ -3912,10 +3898,10 @@
         <v>250</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I7" t="s">
         <v>45</v>
@@ -3938,7 +3924,7 @@
         <v>116</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C8" t="s">
         <v>269</v>
@@ -3956,7 +3942,7 @@
         <v>283</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I8" t="s">
         <v>45</v>
@@ -3979,7 +3965,7 @@
         <v>122</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" t="s">
         <v>269</v>
@@ -3994,10 +3980,10 @@
         <v>254</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I9" t="s">
         <v>45</v>
@@ -4020,7 +4006,7 @@
         <v>128</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C10" t="s">
         <v>269</v>
@@ -4038,7 +4024,7 @@
         <v>284</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I10" t="s">
         <v>45</v>
@@ -4061,7 +4047,7 @@
         <v>134</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C11" t="s">
         <v>269</v>
@@ -4076,10 +4062,10 @@
         <v>258</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I11" t="s">
         <v>45</v>

</xml_diff>